<commit_message>
cost of move is calculated
</commit_message>
<xml_diff>
--- a/thinking.xlsx
+++ b/thinking.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\usefull\java_project\maze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863D9D1A-579D-4B35-B5C8-D9E5100AB3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB14D59-7834-462C-8EF7-B96B9D9D0616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -75,7 +86,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -83,11 +94,146 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -95,6 +241,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -376,15 +549,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="5" max="6" width="7.109375" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -511,7 +686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -519,7 +694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -527,7 +702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -535,7 +710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -543,7 +718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -551,7 +726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -559,7 +734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>6</v>
       </c>
@@ -567,7 +742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>7</v>
       </c>
@@ -575,7 +750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8</v>
       </c>
@@ -583,7 +758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>9</v>
       </c>
@@ -591,12 +766,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>10</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="4">
+        <v>3</v>
+      </c>
+      <c r="F28" s="5">
+        <v>3</v>
+      </c>
+      <c r="G28" s="6">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <f>+E28*F28*G28</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="7">
+        <v>3</v>
+      </c>
+      <c r="F29" s="8">
+        <v>3</v>
+      </c>
+      <c r="G29" s="9">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <f t="shared" ref="H29:H30" si="0">+E29*F29*G29</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E30" s="10">
+        <v>3</v>
+      </c>
+      <c r="F30" s="11">
+        <v>3</v>
+      </c>
+      <c r="G30" s="12">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H31">
+        <f>+H28*H29*H30</f>
+        <v>19683</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complex version is ready as well
</commit_message>
<xml_diff>
--- a/thinking.xlsx
+++ b/thinking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\usefull\java_project\maze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB14D59-7834-462C-8EF7-B96B9D9D0616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D02F60E-13AC-42FD-885A-2B67C1C853AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="10">
   <si>
     <t>Steps</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -233,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -268,6 +277,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,6 +602,7 @@
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="5" max="6" width="7.109375" customWidth="1"/>
     <col min="7" max="7" width="6.5546875" customWidth="1"/>
+    <col min="11" max="15" width="4.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -686,7 +729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>4</v>
       </c>
@@ -694,47 +737,98 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K18" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="N18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K19" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L19" s="22"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="17"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K20" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K21" s="15"/>
+      <c r="L21" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" s="16"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="17"/>
+    </row>
+    <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>5</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K22" s="18"/>
+      <c r="L22" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>6</v>
       </c>
@@ -742,39 +836,82 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>7</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J24" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="N24" s="13"/>
+      <c r="O24" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K25" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L25" s="22"/>
+      <c r="M25" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="N25" s="16"/>
+      <c r="O25" s="17"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>9</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K26" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L26" s="16"/>
+      <c r="M26" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="N26" s="16"/>
+      <c r="O26" s="17"/>
+    </row>
+    <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>10</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K27" s="15"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="N27" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="O27" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E28" s="4">
         <v>3</v>
       </c>
@@ -788,8 +925,19 @@
         <f>+E28*F28*G28</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K28" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="L28" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="M28" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="N28" s="19"/>
+      <c r="O28" s="23"/>
+    </row>
+    <row r="29" spans="1:15" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E29" s="7">
         <v>3</v>
       </c>
@@ -804,7 +952,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E30" s="10">
         <v>3</v>
       </c>
@@ -818,11 +966,71 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J30" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" s="21"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="N30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="O30" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H31">
         <f>+H28*H29*H30</f>
         <v>19683</v>
+      </c>
+      <c r="K31" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L31" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="N31" s="16"/>
+      <c r="O31" s="17"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K32" s="15"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="N32" s="16"/>
+      <c r="O32" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="11:15" x14ac:dyDescent="0.3">
+      <c r="K33" s="15"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="N33" s="22"/>
+      <c r="O33" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="11:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K34" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="N34" s="19"/>
+      <c r="O34" s="23" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some refactoring to make the code more simple
</commit_message>
<xml_diff>
--- a/thinking.xlsx
+++ b/thinking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\usefull\java_project\maze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D02F60E-13AC-42FD-885A-2B67C1C853AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F639007C-BB6D-4678-A87D-10BC27B00548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -242,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -302,13 +302,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -594,7 +591,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,7 +765,7 @@
       <c r="K19" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L19" s="22"/>
+      <c r="L19" s="16"/>
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
       <c r="O19" s="17"/>
@@ -808,7 +805,7 @@
         <v>7</v>
       </c>
       <c r="M21" s="16"/>
-      <c r="N21" s="22"/>
+      <c r="N21" s="16"/>
       <c r="O21" s="17"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -824,7 +821,7 @@
       </c>
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
-      <c r="O22" s="23" t="s">
+      <c r="O22" s="22" t="s">
         <v>7</v>
       </c>
     </row>
@@ -868,7 +865,7 @@
       <c r="K25" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L25" s="22"/>
+      <c r="L25" s="16"/>
       <c r="M25" s="16" t="s">
         <v>7</v>
       </c>
@@ -904,7 +901,7 @@
       <c r="M27" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="N27" s="22" t="s">
+      <c r="N27" s="16" t="s">
         <v>7</v>
       </c>
       <c r="O27" s="17" t="s">
@@ -913,17 +910,17 @@
     </row>
     <row r="28" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E28" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F28" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G28" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H28">
         <f>+E28*F28*G28</f>
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="K28" s="18" t="s">
         <v>7</v>
@@ -935,36 +932,36 @@
         <v>7</v>
       </c>
       <c r="N28" s="19"/>
-      <c r="O28" s="23"/>
+      <c r="O28" s="22"/>
     </row>
     <row r="29" spans="1:15" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E29" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F29" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G29" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H29">
         <f t="shared" ref="H29:H30" si="0">+E29*F29*G29</f>
-        <v>27</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E30" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F30" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G30" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H30">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="J30" t="s">
         <v>9</v>
@@ -984,12 +981,12 @@
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H31">
         <f>+H28*H29*H30</f>
-        <v>19683</v>
+        <v>262144</v>
       </c>
       <c r="K31" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L31" s="22" t="s">
+      <c r="L31" s="16" t="s">
         <v>7</v>
       </c>
       <c r="M31" s="16" t="s">
@@ -1015,7 +1012,7 @@
       <c r="M33" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="N33" s="22"/>
+      <c r="N33" s="16"/>
       <c r="O33" s="17" t="s">
         <v>7</v>
       </c>
@@ -1029,7 +1026,7 @@
         <v>7</v>
       </c>
       <c r="N34" s="19"/>
-      <c r="O34" s="23" t="s">
+      <c r="O34" s="22" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>